<commit_message>
update spearman summarizing script and results
</commit_message>
<xml_diff>
--- a/summary_spearman_1000.xlsx
+++ b/summary_spearman_1000.xlsx
@@ -500,22 +500,22 @@
       <c r="B2" s="1" t="inlineStr"/>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>MPSP [$/gal]</t>
+          <t>MPSP</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>Product GWP disp [kg CO2/gal]</t>
+          <t>GWP</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>MPSP [$/gal]</t>
+          <t>MPSP</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>Product GWP disp [kg CO2/gal]</t>
+          <t>GWP</t>
         </is>
       </c>
     </row>
@@ -545,15 +545,11 @@
       <c r="C4" t="n">
         <v>0.9392075672075674</v>
       </c>
-      <c r="D4" t="n">
-        <v>0.05422560622560623</v>
-      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="n">
         <v>0.9395858075858076</v>
       </c>
-      <c r="F4" t="n">
-        <v>0.04815427215427216</v>
-      </c>
+      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n"/>
@@ -562,15 +558,11 @@
           <t>Corn CF [kg CO2/kg]</t>
         </is>
       </c>
-      <c r="C5" t="n">
-        <v>0.04473874473874474</v>
-      </c>
+      <c r="C5" t="inlineStr"/>
       <c r="D5" t="n">
         <v>0.73594821994822</v>
       </c>
-      <c r="E5" t="n">
-        <v>0.04126463326463326</v>
-      </c>
+      <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
         <v>0.7371539091539092</v>
       </c>
@@ -578,49 +570,41 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Stream-DDGS</t>
+          <t>Stream-steam</t>
         </is>
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>DDGS CF [kg CO2/kg]</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>-0.02338748338748339</v>
-      </c>
+          <t>Steam CF [kg CO2/kg]</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
       <c r="D6" t="n">
-        <v>-0.5902128022128023</v>
-      </c>
-      <c r="E6" t="n">
-        <v>-0.02244625044625045</v>
-      </c>
+        <v>0.2622401022401022</v>
+      </c>
+      <c r="E6" t="inlineStr"/>
       <c r="F6" t="n">
-        <v>-0.594985542985543</v>
+        <v>0.2665123465123465</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Stream-steam</t>
+          <t>Stream-DDGS</t>
         </is>
       </c>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>Steam CF [kg CO2/kg]</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>0.04511210111210111</v>
-      </c>
+          <t>DDGS CF [kg CO2/kg]</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
       <c r="D7" t="n">
-        <v>0.2622401022401022</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.04566467766467766</v>
-      </c>
+        <v>-0.5902128022128023</v>
+      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="n">
-        <v>0.2665123465123465</v>
+        <v>-0.594985542985543</v>
       </c>
     </row>
     <row r="8">
@@ -634,15 +618,11 @@
           <t>Natural gas CF [kg CO2/kg]</t>
         </is>
       </c>
-      <c r="C8" t="n">
-        <v>0.01556993156993157</v>
-      </c>
+      <c r="C8" t="inlineStr"/>
       <c r="D8" t="n">
         <v>0.2332697692697693</v>
       </c>
-      <c r="E8" t="n">
-        <v>0.01344036144036144</v>
-      </c>
+      <c r="E8" t="inlineStr"/>
       <c r="F8" t="n">
         <v>0.2340793140793141</v>
       </c>
@@ -690,22 +670,22 @@
       <c r="B2" s="1" t="inlineStr"/>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>MPSP [$/gal]</t>
+          <t>MPSP</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>Product GWP disp [kg CO2/gal]</t>
+          <t>GWP</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>MPSP [$/gal]</t>
+          <t>MPSP</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>Product GWP disp [kg CO2/gal]</t>
+          <t>GWP</t>
         </is>
       </c>
     </row>
@@ -735,15 +715,11 @@
       <c r="C4" t="n">
         <v>0.8537019017019017</v>
       </c>
-      <c r="D4" t="n">
-        <v>0.0135033975033975</v>
-      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="n">
         <v>0.8522028722028723</v>
       </c>
-      <c r="F4" t="n">
-        <v>0.01971311571311572</v>
-      </c>
+      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -759,15 +735,11 @@
       <c r="C5" t="n">
         <v>-0.266984462984463</v>
       </c>
-      <c r="D5" t="n">
-        <v>0.03546064746064746</v>
-      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="n">
         <v>-0.2831955911955912</v>
       </c>
-      <c r="F5" t="n">
-        <v>0.03269134469134469</v>
-      </c>
+      <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -783,15 +755,11 @@
       <c r="C6" t="n">
         <v>-0.2446337326337326</v>
       </c>
-      <c r="D6" t="n">
-        <v>-0.04868684468684469</v>
-      </c>
+      <c r="D6" t="inlineStr"/>
       <c r="E6" t="n">
         <v>-0.2575972255972256</v>
       </c>
-      <c r="F6" t="n">
-        <v>-0.04655439455439456</v>
-      </c>
+      <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -824,15 +792,11 @@
           <t>Turbogenerator efficiency [-]</t>
         </is>
       </c>
-      <c r="C8" t="n">
-        <v>-0.1223271383271383</v>
-      </c>
+      <c r="C8" t="inlineStr"/>
       <c r="D8" t="n">
         <v>-0.2733119493119494</v>
       </c>
-      <c r="E8" t="n">
-        <v>-0.1252021492021492</v>
-      </c>
+      <c r="E8" t="inlineStr"/>
       <c r="F8" t="n">
         <v>-0.2764343404343405</v>
       </c>
@@ -848,15 +812,11 @@
           <t>Sugarcane CF [kg CO2/kg]</t>
         </is>
       </c>
-      <c r="C9" t="n">
-        <v>0.05013201813201813</v>
-      </c>
+      <c r="C9" t="inlineStr"/>
       <c r="D9" t="n">
         <v>0.2129309369309369</v>
       </c>
-      <c r="E9" t="n">
-        <v>0.05232308832308833</v>
-      </c>
+      <c r="E9" t="inlineStr"/>
       <c r="F9" t="n">
         <v>0.205964497964498</v>
       </c>
@@ -872,15 +832,11 @@
           <t>Electricity production CF [kg CO2/kWh]</t>
         </is>
       </c>
-      <c r="C10" t="n">
-        <v>-6.565206565206567e-05</v>
-      </c>
+      <c r="C10" t="inlineStr"/>
       <c r="D10" t="n">
         <v>-0.5327549087549087</v>
       </c>
-      <c r="E10" t="n">
-        <v>0.005691641691641692</v>
-      </c>
+      <c r="E10" t="inlineStr"/>
       <c r="F10" t="n">
         <v>-0.5421264621264622</v>
       </c>
@@ -928,22 +884,22 @@
       <c r="B2" s="1" t="inlineStr"/>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>MPSP [$/gal]</t>
+          <t>MPSP</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>Product GWP disp [kg CO2/gal]</t>
+          <t>GWP</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>MPSP [$/gal]</t>
+          <t>MPSP</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>Product GWP disp [kg CO2/gal]</t>
+          <t>GWP</t>
         </is>
       </c>
     </row>
@@ -973,15 +929,11 @@
       <c r="C4" t="n">
         <v>0.5833406833406835</v>
       </c>
-      <c r="D4" t="n">
-        <v>-0.04660448260448261</v>
-      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="n">
         <v>0.5806122406122406</v>
       </c>
-      <c r="F4" t="n">
-        <v>-0.04631827031827032</v>
-      </c>
+      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -997,15 +949,11 @@
       <c r="C5" t="n">
         <v>-0.4336618216618217</v>
       </c>
-      <c r="D5" t="n">
-        <v>0.006782094782094783</v>
-      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="n">
         <v>-0.4402746682746683</v>
       </c>
-      <c r="F5" t="n">
-        <v>0.005533829533829534</v>
-      </c>
+      <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -1021,15 +969,11 @@
       <c r="C6" t="n">
         <v>-0.2955820515820516</v>
       </c>
-      <c r="D6" t="n">
-        <v>0.08633532233532235</v>
-      </c>
+      <c r="D6" t="inlineStr"/>
       <c r="E6" t="n">
         <v>-0.2931759891759892</v>
       </c>
-      <c r="F6" t="n">
-        <v>0.07848210648210649</v>
-      </c>
+      <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n"/>
@@ -1065,15 +1009,11 @@
       <c r="C8" t="n">
         <v>-0.2857920937920938</v>
       </c>
-      <c r="D8" t="n">
-        <v>-0.002230802230802231</v>
-      </c>
+      <c r="D8" t="inlineStr"/>
       <c r="E8" t="n">
         <v>-0.2851132291132292</v>
       </c>
-      <c r="F8" t="n">
-        <v>-0.0001035241035241035</v>
-      </c>
+      <c r="F8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -1089,15 +1029,11 @@
       <c r="C9" t="n">
         <v>-0.2429263229263229</v>
       </c>
-      <c r="D9" t="n">
-        <v>-0.01008514608514608</v>
-      </c>
+      <c r="D9" t="inlineStr"/>
       <c r="E9" t="n">
         <v>-0.2508716868716869</v>
       </c>
-      <c r="F9" t="n">
-        <v>-0.007774075774075775</v>
-      </c>
+      <c r="F9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -1134,15 +1070,11 @@
           <t>Electricity production CF [kg CO2/kWh]</t>
         </is>
       </c>
-      <c r="C11" t="n">
-        <v>0.0133981813981814</v>
-      </c>
+      <c r="C11" t="inlineStr"/>
       <c r="D11" t="n">
         <v>-0.3733970893970894</v>
       </c>
-      <c r="E11" t="n">
-        <v>0.01319439719439719</v>
-      </c>
+      <c r="E11" t="inlineStr"/>
       <c r="F11" t="n">
         <v>-0.3693773013773014</v>
       </c>
@@ -1190,22 +1122,22 @@
       <c r="B2" s="1" t="inlineStr"/>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>MPSP [$/gal]</t>
+          <t>MPSP</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>Product GWP disp [kg CO2/gal]</t>
+          <t>GWP</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>MPSP [$/gal]</t>
+          <t>MPSP</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>Product GWP disp [kg CO2/gal]</t>
+          <t>GWP</t>
         </is>
       </c>
     </row>
@@ -1235,15 +1167,11 @@
       <c r="C4" t="n">
         <v>0.5421585720400194</v>
       </c>
-      <c r="D4" t="n">
-        <v>0.04294243814725102</v>
-      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="n">
         <v>0.5403094803094803</v>
       </c>
-      <c r="F4" t="n">
-        <v>0.02613839013839014</v>
-      </c>
+      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -1259,15 +1187,11 @@
       <c r="C5" t="n">
         <v>0.5035866720729146</v>
       </c>
-      <c r="D5" t="n">
-        <v>-0.02174133221200371</v>
-      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="n">
         <v>0.4911772431772432</v>
       </c>
-      <c r="F5" t="n">
-        <v>0.005540621540621541</v>
-      </c>
+      <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n"/>
@@ -1279,15 +1203,11 @@
       <c r="C6" t="n">
         <v>-0.3295304796587641</v>
       </c>
-      <c r="D6" t="n">
-        <v>-0.0631882504969296</v>
-      </c>
+      <c r="D6" t="inlineStr"/>
       <c r="E6" t="n">
         <v>-0.2447606447606447</v>
       </c>
-      <c r="F6" t="n">
-        <v>-0.06366848766848766</v>
-      </c>
+      <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -1327,15 +1247,11 @@
       <c r="C8" t="n">
         <v>0.2550524735121744</v>
       </c>
-      <c r="D8" t="n">
-        <v>-0.0510253026753071</v>
-      </c>
+      <c r="D8" t="inlineStr"/>
       <c r="E8" t="n">
         <v>0.239924675924676</v>
       </c>
-      <c r="F8" t="n">
-        <v>-0.04184693384693385</v>
-      </c>
+      <c r="F8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -1372,15 +1288,11 @@
           <t>PT solids loading [-]</t>
         </is>
       </c>
-      <c r="C10" t="n">
-        <v>-0.1120660213555905</v>
-      </c>
+      <c r="C10" t="inlineStr"/>
       <c r="D10" t="n">
         <v>-0.2675112904388318</v>
       </c>
-      <c r="E10" t="n">
-        <v>-0.09528592728592729</v>
-      </c>
+      <c r="E10" t="inlineStr"/>
       <c r="F10" t="n">
         <v>-0.2286495246495247</v>
       </c>
@@ -1396,15 +1308,11 @@
           <t>Turbogenerator efficiency [-]</t>
         </is>
       </c>
-      <c r="C11" t="n">
-        <v>-0.09853845136955813</v>
-      </c>
+      <c r="C11" t="inlineStr"/>
       <c r="D11" t="n">
         <v>-0.2485275716939876</v>
       </c>
-      <c r="E11" t="n">
-        <v>-0.1106001746001746</v>
-      </c>
+      <c r="E11" t="inlineStr"/>
       <c r="F11" t="n">
         <v>-0.2538399378399379</v>
       </c>
@@ -1420,15 +1328,11 @@
           <t>Electricity production CF [kg CO2/kWh]</t>
         </is>
       </c>
-      <c r="C12" t="n">
-        <v>-0.01953870175581226</v>
-      </c>
+      <c r="C12" t="inlineStr"/>
       <c r="D12" t="n">
         <v>-0.3407409178620361</v>
       </c>
-      <c r="E12" t="n">
-        <v>-0.03046137046137046</v>
-      </c>
+      <c r="E12" t="inlineStr"/>
       <c r="F12" t="n">
         <v>-0.4242194682194683</v>
       </c>
@@ -1445,9 +1349,7 @@
       <c r="E13" t="n">
         <v>-0.2613142293142294</v>
       </c>
-      <c r="F13" t="n">
-        <v>0.008307272307272308</v>
-      </c>
+      <c r="F13" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1493,22 +1395,22 @@
       <c r="B2" s="1" t="inlineStr"/>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>MPSP [$/gal]</t>
+          <t>MPSP</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>Product GWP disp [kg CO2/gal]</t>
+          <t>GWP</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>MPSP [$/gal]</t>
+          <t>MPSP</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>Product GWP disp [kg CO2/gal]</t>
+          <t>GWP</t>
         </is>
       </c>
     </row>
@@ -1538,15 +1440,11 @@
       <c r="C4" t="n">
         <v>-0.5689743707642609</v>
       </c>
-      <c r="D4" t="n">
-        <v>0.03205548688515574</v>
-      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="n">
         <v>-0.5526342150242372</v>
       </c>
-      <c r="F4" t="n">
-        <v>0.02404165148925439</v>
-      </c>
+      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -1586,15 +1484,11 @@
       <c r="C6" t="n">
         <v>0.4462724775348618</v>
       </c>
-      <c r="D6" t="n">
-        <v>-0.02305641280857728</v>
-      </c>
+      <c r="D6" t="inlineStr"/>
       <c r="E6" t="n">
         <v>0.4296826753341365</v>
       </c>
-      <c r="F6" t="n">
-        <v>-0.03547325506458573</v>
-      </c>
+      <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -1610,15 +1504,11 @@
       <c r="C7" t="n">
         <v>-0.3676806024001882</v>
       </c>
-      <c r="D7" t="n">
-        <v>-0.001151462859832144</v>
-      </c>
+      <c r="D7" t="inlineStr"/>
       <c r="E7" t="n">
         <v>-0.3776613942671411</v>
       </c>
-      <c r="F7" t="n">
-        <v>-0.03271045233358551</v>
-      </c>
+      <c r="F7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -1658,9 +1548,7 @@
       <c r="C9" t="n">
         <v>-0.22915243296071</v>
       </c>
-      <c r="D9" t="n">
-        <v>0.07391451031092815</v>
-      </c>
+      <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
     </row>
@@ -1675,15 +1563,11 @@
           <t>Boiler efficiency [-]</t>
         </is>
       </c>
-      <c r="C10" t="n">
-        <v>-0.08376922057443316</v>
-      </c>
+      <c r="C10" t="inlineStr"/>
       <c r="D10" t="n">
         <v>-0.3191129527400391</v>
       </c>
-      <c r="E10" t="n">
-        <v>-0.1040467417598326</v>
-      </c>
+      <c r="E10" t="inlineStr"/>
       <c r="F10" t="n">
         <v>-0.3181659615007424</v>
       </c>
@@ -1730,22 +1614,22 @@
       <c r="B2" s="1" t="inlineStr"/>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>MPSP [$/gal]</t>
+          <t>MPSP</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>Product GWP disp [kg CO2/gal]</t>
+          <t>GWP</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>MPSP [$/gal]</t>
+          <t>MPSP</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>Product GWP disp [kg CO2/gal]</t>
+          <t>GWP</t>
         </is>
       </c>
     </row>
@@ -1775,15 +1659,11 @@
       <c r="C4" t="n">
         <v>-0.4826326130837554</v>
       </c>
-      <c r="D4" t="n">
-        <v>0.09556885504467892</v>
-      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="n">
         <v>-0.4769592745914514</v>
       </c>
-      <c r="F4" t="n">
-        <v>0.06932463969509745</v>
-      </c>
+      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -1799,15 +1679,11 @@
       <c r="C5" t="n">
         <v>0.412132557924584</v>
       </c>
-      <c r="D5" t="n">
-        <v>0.01663250276541251</v>
-      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="n">
         <v>0.4068547746982931</v>
       </c>
-      <c r="F5" t="n">
-        <v>-0.01050673941797596</v>
-      </c>
+      <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -1823,15 +1699,11 @@
       <c r="C6" t="n">
         <v>-0.3624249760728459</v>
       </c>
-      <c r="D6" t="n">
-        <v>0.02253274516760934</v>
-      </c>
+      <c r="D6" t="inlineStr"/>
       <c r="E6" t="n">
         <v>-0.3450721843396352</v>
       </c>
-      <c r="F6" t="n">
-        <v>0.04273559820849198</v>
-      </c>
+      <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -1895,15 +1767,11 @@
       <c r="C9" t="n">
         <v>-0.2941093731831016</v>
       </c>
-      <c r="D9" t="n">
-        <v>-0.04127463900558449</v>
-      </c>
+      <c r="D9" t="inlineStr"/>
       <c r="E9" t="n">
         <v>-0.2933912593119891</v>
       </c>
-      <c r="F9" t="n">
-        <v>0.0007189409008507291</v>
-      </c>
+      <c r="F9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -1940,15 +1808,11 @@
           <t>Boiler efficiency [-]</t>
         </is>
       </c>
-      <c r="C11" t="n">
-        <v>-0.05292619404698368</v>
-      </c>
+      <c r="C11" t="inlineStr"/>
       <c r="D11" t="n">
         <v>-0.3407287122867799</v>
       </c>
-      <c r="E11" t="n">
-        <v>-0.1045787399942078</v>
-      </c>
+      <c r="E11" t="inlineStr"/>
       <c r="F11" t="n">
         <v>-0.3520451875999212</v>
       </c>
@@ -1995,22 +1859,22 @@
       <c r="B2" s="1" t="inlineStr"/>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>MPSP [$/kg]</t>
+          <t>MPSP</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>Product GWP disp [kg CO2/kg]</t>
+          <t>GWP</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>MPSP [$/kg]</t>
+          <t>MPSP</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>Product GWP disp [kg CO2/kg]</t>
+          <t>GWP</t>
         </is>
       </c>
     </row>
@@ -2040,15 +1904,11 @@
       <c r="C4" t="n">
         <v>-0.6077200163733114</v>
       </c>
-      <c r="D4" t="n">
-        <v>-0.1704300817254082</v>
-      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="n">
         <v>-0.4579101714076755</v>
       </c>
-      <c r="F4" t="n">
-        <v>-0.09002090602516587</v>
-      </c>
+      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -2064,9 +1924,7 @@
       <c r="C5" t="n">
         <v>-0.3395446525611529</v>
       </c>
-      <c r="D5" t="n">
-        <v>-0.165722754668511</v>
-      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
     </row>
@@ -2084,15 +1942,11 @@
       <c r="C6" t="n">
         <v>-0.3354420088359422</v>
       </c>
-      <c r="D6" t="n">
-        <v>0.05069628918655695</v>
-      </c>
+      <c r="D6" t="inlineStr"/>
       <c r="E6" t="n">
         <v>-0.283895167860266</v>
       </c>
-      <c r="F6" t="n">
-        <v>-0.04454349754204644</v>
-      </c>
+      <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -2108,9 +1962,7 @@
       <c r="C7" t="n">
         <v>0.291282623117422</v>
       </c>
-      <c r="D7" t="n">
-        <v>0.05377475404745437</v>
-      </c>
+      <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
     </row>
@@ -2128,15 +1980,11 @@
       <c r="C8" t="n">
         <v>0.2713647719734075</v>
       </c>
-      <c r="D8" t="n">
-        <v>-0.004742614366169351</v>
-      </c>
+      <c r="D8" t="inlineStr"/>
       <c r="E8" t="n">
         <v>0.2384258154758671</v>
       </c>
-      <c r="F8" t="n">
-        <v>0.03060776805855506</v>
-      </c>
+      <c r="F8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -2152,9 +2000,7 @@
       <c r="C9" t="n">
         <v>0.2336700213135348</v>
       </c>
-      <c r="D9" t="n">
-        <v>0.01299532796025238</v>
-      </c>
+      <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
     </row>
@@ -2165,15 +2011,11 @@
           <t>Natural gas CF [kg CO2/kg]</t>
         </is>
       </c>
-      <c r="C10" t="n">
-        <v>-0.007503775742092113</v>
-      </c>
+      <c r="C10" t="inlineStr"/>
       <c r="D10" t="n">
         <v>0.5414608946038646</v>
       </c>
-      <c r="E10" t="n">
-        <v>-0.01317344679843806</v>
-      </c>
+      <c r="E10" t="inlineStr"/>
       <c r="F10" t="n">
         <v>0.4307638511228082</v>
       </c>
@@ -2189,15 +2031,11 @@
           <t>Boiler efficiency [-]</t>
         </is>
       </c>
-      <c r="C11" t="n">
-        <v>-0.03505864750801022</v>
-      </c>
+      <c r="C11" t="inlineStr"/>
       <c r="D11" t="n">
         <v>-0.4663006196451508</v>
       </c>
-      <c r="E11" t="n">
-        <v>-0.08893021544952048</v>
-      </c>
+      <c r="E11" t="inlineStr"/>
       <c r="F11" t="n">
         <v>-0.3431964569021264</v>
       </c>
@@ -2218,9 +2056,7 @@
       <c r="E12" t="n">
         <v>-0.2014706433870472</v>
       </c>
-      <c r="F12" t="n">
-        <v>-0.05074818162595151</v>
-      </c>
+      <c r="F12" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>